<commit_message>
masih menghilangkan array pertama....
</commit_message>
<xml_diff>
--- a/public/files/template/inventory/lap_bhp_pengadaan.xlsx
+++ b/public/files/template/inventory/lap_bhp_pengadaan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="63">
   <si>
     <t>No.</t>
   </si>
@@ -96,9 +96,6 @@
     <t>[a.harga_akhir]</t>
   </si>
   <si>
-    <t>[a.jmlbaik]</t>
-  </si>
-  <si>
     <t>dari [b.tgl1] s/d [b.tgl2]</t>
   </si>
   <si>
@@ -169,6 +166,48 @@
   </si>
   <si>
     <t>[a.harga_beli2]</t>
+  </si>
+  <si>
+    <t>[a.total1]</t>
+  </si>
+  <si>
+    <t>[a.total2]</t>
+  </si>
+  <si>
+    <t>[a.total3]</t>
+  </si>
+  <si>
+    <t>[a.total4]</t>
+  </si>
+  <si>
+    <t>[a.total5]</t>
+  </si>
+  <si>
+    <t>[a.total7]</t>
+  </si>
+  <si>
+    <t>[a.total6]</t>
+  </si>
+  <si>
+    <t>[a.total8]</t>
+  </si>
+  <si>
+    <t>[a.total12]</t>
+  </si>
+  <si>
+    <t>[a.total11]</t>
+  </si>
+  <si>
+    <t>[a.total10]</t>
+  </si>
+  <si>
+    <t>[a.total9]</t>
+  </si>
+  <si>
+    <t>[a.nilaiaset]</t>
+  </si>
+  <si>
+    <t>[a.totaljumlah]</t>
   </si>
 </sst>
 </file>
@@ -438,37 +477,37 @@
     <xf numFmtId="3" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -866,37 +905,39 @@
   <dimension ref="A1:AS10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="26.140625" customWidth="1"/>
     <col min="3" max="3" width="14.28515625" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="7" max="9" width="9.140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:45" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="29"/>
+      <c r="A1" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
       <c r="R1" s="8"/>
       <c r="S1" s="8"/>
       <c r="T1" s="8"/>
@@ -905,25 +946,25 @@
       <c r="AR1" s="1"/>
     </row>
     <row r="2" spans="1:45" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="29"/>
+      <c r="A2" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="27"/>
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
@@ -1029,54 +1070,54 @@
       <c r="AR6" s="1"/>
     </row>
     <row r="7" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="32" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="34" t="s">
+      <c r="E7" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="27" t="s">
+      <c r="G7" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="28"/>
+      <c r="H7" s="37"/>
       <c r="I7" s="4"/>
-      <c r="J7" s="27">
+      <c r="J7" s="36">
         <v>42005</v>
       </c>
-      <c r="K7" s="28"/>
+      <c r="K7" s="37"/>
       <c r="L7" s="4">
         <v>1</v>
       </c>
-      <c r="M7" s="27" t="s">
+      <c r="M7" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="N7" s="28"/>
+      <c r="N7" s="37"/>
       <c r="O7" s="5">
         <v>2</v>
       </c>
-      <c r="P7" s="27" t="s">
+      <c r="P7" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="Q7" s="28"/>
+      <c r="Q7" s="37"/>
       <c r="R7" s="5">
         <v>3</v>
       </c>
-      <c r="S7" s="27">
+      <c r="S7" s="36">
         <v>42095</v>
       </c>
-      <c r="T7" s="28"/>
+      <c r="T7" s="37"/>
       <c r="U7" s="5">
         <v>4</v>
       </c>
@@ -1138,14 +1179,14 @@
       </c>
     </row>
     <row r="8" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A8" s="31"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="35"/>
+      <c r="A8" s="29"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="33"/>
       <c r="D8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
       <c r="G8" s="10" t="s">
         <v>16</v>
       </c>
@@ -1361,141 +1402,127 @@
         <v>24</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="20" t="e">
-        <f>D10*E10</f>
-        <v>#VALUE!</v>
+        <v>62</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>61</v>
       </c>
       <c r="G10" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="H10" s="20" t="s">
+      <c r="I10" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="J10" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="K10" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="L10" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="M10" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="N10" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="O10" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="P10" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q10" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="R10" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="S10" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="T10" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="U10" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="V10" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="W10" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="X10" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y10" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z10" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA10" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB10" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC10" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD10" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE10" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF10" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="AG10" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH10" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="AI10" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ10" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK10" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL10" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="AM10" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="AN10" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="AO10" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="AP10" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="AQ10" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="I10" s="20" t="e">
-        <f>(G10*H10)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="J10" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="K10" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="L10" s="20" t="e">
-        <f t="shared" ref="L10" si="0">(J10*K10)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M10" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="N10" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="O10" s="20" t="e">
-        <f t="shared" ref="O10" si="1">(M10*N10)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="P10" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q10" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="R10" s="20" t="e">
-        <f t="shared" ref="R10" si="2">(P10*Q10)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S10" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="T10" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="U10" s="20" t="e">
-        <f t="shared" ref="U10" si="3">(S10*T10)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="V10" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="W10" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="X10" s="20" t="e">
-        <f t="shared" ref="X10" si="4">(V10*W10)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Y10" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="Z10" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA10" s="20" t="e">
-        <f t="shared" ref="AA10" si="5">(Y10*Z10)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AB10" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC10" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="AD10" s="20" t="e">
-        <f t="shared" ref="AD10" si="6">(AB10*AC10)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AE10" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="AF10" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="AG10" s="20" t="e">
-        <f t="shared" ref="AG10" si="7">(AE10*AF10)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AH10" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="AI10" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="AJ10" s="20" t="e">
-        <f t="shared" ref="AJ10" si="8">(AH10*AI10)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AK10" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="AL10" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="AM10" s="20" t="e">
-        <f t="shared" ref="AM10" si="9">(AK10*AL10)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AN10" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="AO10" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="AP10" s="20" t="e">
-        <f t="shared" ref="AP10" si="10">(AN10*AO10)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AQ10" s="20" t="s">
+      <c r="AR10" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="AR10" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="AS10" s="20" t="e">
-        <f t="shared" ref="AS10" si="11">(AQ10*AR10)</f>
-        <v>#VALUE!</v>
+      <c r="AS10" s="20" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>